<commit_message>
change column name, etc
Changed Stenolophus thoracicus to Agonoleptus thoracicus (changed column name in the excel and csv files). Tried to create a distance matrix between sites in the map.
</commit_message>
<xml_diff>
--- a/PNR_Raw_Data/PNR_ENV_2022.xlsx
+++ b/PNR_Raw_Data/PNR_ENV_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27424"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/perry_1864_osu_edu/Documents/Documents/Perry Lab/Powdermill Nature Reserve/PNR_Beetles/PNR Raw Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32f02f1096a9313f/Documents/Entomology MS/Thesis research/PNR_Beetles_github_folder/PNR_Raw_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A58FFDF3-DFA9-4F47-8168-BBA5BBFEC40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{A58FFDF3-DFA9-4F47-8168-BBA5BBFEC40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2349646D-2AE0-49D0-9019-41A78461603D}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{CA8C2220-5D77-4368-A0A9-BCAE7FCA22D1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{CA8C2220-5D77-4368-A0A9-BCAE7FCA22D1}"/>
   </bookViews>
   <sheets>
     <sheet name="DENSI" sheetId="1" r:id="rId1"/>
@@ -207,7 +207,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,9 +301,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -341,7 +341,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -447,7 +447,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -589,7 +589,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -603,18 +603,18 @@
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="8.81640625" style="1"/>
     <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="8.85546875" style="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="8.81640625" style="1"/>
+    <col min="9" max="9" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -646,7 +646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
@@ -676,7 +676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
@@ -706,7 +706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -736,7 +736,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
@@ -766,7 +766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -796,7 +796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -826,7 +826,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
@@ -856,7 +856,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -886,7 +886,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -916,7 +916,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
@@ -946,7 +946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
@@ -976,7 +976,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
         <v>10</v>
       </c>
@@ -1376,33 +1376,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD38425-E846-4376-8DFE-C36F511B0F31}">
   <dimension ref="A1:Y97"/>
   <sheetViews>
-    <sheetView topLeftCell="I67" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
+    <sheetView topLeftCell="H76" workbookViewId="0">
+      <selection activeCell="V86" sqref="V86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="8.81640625" style="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="1"/>
-    <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="1"/>
-    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
-    <col min="10" max="11" width="8.85546875" style="1"/>
-    <col min="12" max="12" width="9.42578125" style="1" customWidth="1"/>
-    <col min="13" max="14" width="8.85546875" style="1"/>
-    <col min="15" max="15" width="9.140625" style="1" customWidth="1"/>
-    <col min="16" max="17" width="8.85546875" style="1"/>
-    <col min="18" max="18" width="9.140625" style="1" customWidth="1"/>
-    <col min="19" max="20" width="8.85546875" style="1"/>
-    <col min="21" max="21" width="9.140625" style="1" customWidth="1"/>
-    <col min="22" max="23" width="8.85546875" style="6"/>
-    <col min="24" max="24" width="10.28515625" style="6" customWidth="1"/>
-    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.81640625" style="1"/>
+    <col min="6" max="6" width="9.1796875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="8.81640625" style="1"/>
+    <col min="9" max="9" width="8.7265625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="8.81640625" style="1"/>
+    <col min="12" max="12" width="9.453125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="8.81640625" style="1"/>
+    <col min="15" max="15" width="9.1796875" style="1" customWidth="1"/>
+    <col min="16" max="17" width="8.81640625" style="1"/>
+    <col min="18" max="18" width="9.1796875" style="1" customWidth="1"/>
+    <col min="19" max="20" width="8.81640625" style="1"/>
+    <col min="21" max="21" width="9.1796875" style="1" customWidth="1"/>
+    <col min="22" max="23" width="8.81640625" style="6"/>
+    <col min="24" max="24" width="10.26953125" style="6" customWidth="1"/>
+    <col min="25" max="25" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -5007,7 +5007,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>6</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
@@ -5847,7 +5847,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>10</v>
       </c>
@@ -5931,7 +5931,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>6</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>10</v>
       </c>
@@ -6183,7 +6183,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>6</v>
       </c>
@@ -6267,7 +6267,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>10</v>
       </c>
@@ -6351,7 +6351,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -6435,7 +6435,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>10</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>6</v>
       </c>
@@ -6603,7 +6603,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>10</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -6771,7 +6771,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>10</v>
       </c>
@@ -6855,7 +6855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>6</v>
       </c>
@@ -6939,7 +6939,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>10</v>
       </c>
@@ -7023,7 +7023,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>7</v>
       </c>
@@ -7107,7 +7107,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>10</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>6</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>10</v>
       </c>
@@ -7359,7 +7359,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>7</v>
       </c>
@@ -7443,7 +7443,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>10</v>
       </c>
@@ -7527,7 +7527,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>10</v>
       </c>
@@ -7611,7 +7611,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>6</v>
       </c>
@@ -7695,7 +7695,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="1:25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
@@ -7779,7 +7779,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>10</v>
       </c>
@@ -7863,7 +7863,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>10</v>
       </c>
@@ -7947,7 +7947,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>6</v>
       </c>
@@ -8031,7 +8031,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="1:25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
@@ -8115,7 +8115,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>10</v>
       </c>
@@ -8199,7 +8199,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="82" spans="1:25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>6</v>
       </c>
@@ -8283,7 +8283,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="83" spans="1:25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>10</v>
       </c>
@@ -8367,7 +8367,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>7</v>
       </c>
@@ -8451,7 +8451,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>10</v>
       </c>
@@ -8535,7 +8535,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="86" spans="1:25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>6</v>
       </c>
@@ -8619,7 +8619,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>10</v>
       </c>
@@ -8703,7 +8703,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>7</v>
       </c>
@@ -8787,7 +8787,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>10</v>
       </c>
@@ -8871,7 +8871,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="90" spans="1:25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>6</v>
       </c>
@@ -8955,7 +8955,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="91" spans="1:25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>10</v>
       </c>
@@ -9039,7 +9039,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="1:25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>7</v>
       </c>
@@ -9123,7 +9123,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="93" spans="1:25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>10</v>
       </c>
@@ -9207,7 +9207,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>6</v>
       </c>
@@ -9291,7 +9291,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="95" spans="1:25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>10</v>
       </c>
@@ -9375,7 +9375,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>7</v>
       </c>
@@ -9459,7 +9459,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="97" spans="1:25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>10</v>
       </c>
@@ -9556,21 +9556,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38461446-62E5-46CD-9F86-3B429A81B9D7}">
   <dimension ref="A1:H193"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I195" sqref="I195"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.1796875" style="1"/>
+    <col min="4" max="4" width="14.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" style="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -9596,7 +9596,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -9623,7 +9623,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -9650,7 +9650,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -9677,7 +9677,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -9704,7 +9704,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -9731,7 +9731,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -9758,7 +9758,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -9785,7 +9785,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -9812,7 +9812,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -9839,7 +9839,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -9866,7 +9866,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -9893,7 +9893,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -9920,7 +9920,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -9947,7 +9947,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -9974,7 +9974,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -10001,7 +10001,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -10028,7 +10028,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -10055,7 +10055,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -10082,7 +10082,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -10109,7 +10109,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -10136,7 +10136,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -10163,7 +10163,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -10190,7 +10190,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -10217,7 +10217,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -10244,7 +10244,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -10271,7 +10271,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -10298,7 +10298,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -10325,7 +10325,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -10352,7 +10352,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -10379,7 +10379,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -10406,7 +10406,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -10433,7 +10433,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -10460,7 +10460,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
@@ -10487,7 +10487,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -10514,7 +10514,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -10541,7 +10541,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -10568,7 +10568,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -10595,7 +10595,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
@@ -10622,7 +10622,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
@@ -10649,7 +10649,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -10676,7 +10676,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
@@ -10703,7 +10703,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -10730,7 +10730,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
@@ -10757,7 +10757,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
@@ -10784,7 +10784,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
@@ -10811,7 +10811,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
@@ -10838,7 +10838,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -10865,7 +10865,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
@@ -10892,7 +10892,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
@@ -10919,7 +10919,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>6</v>
       </c>
@@ -10946,7 +10946,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -10973,7 +10973,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
@@ -11000,7 +11000,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>10</v>
       </c>
@@ -11027,7 +11027,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>6</v>
       </c>
@@ -11054,7 +11054,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -11081,7 +11081,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>10</v>
       </c>
@@ -11108,7 +11108,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>6</v>
       </c>
@@ -11135,7 +11135,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>10</v>
       </c>
@@ -11162,7 +11162,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -11189,7 +11189,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>10</v>
       </c>
@@ -11216,7 +11216,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>6</v>
       </c>
@@ -11243,7 +11243,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>10</v>
       </c>
@@ -11270,7 +11270,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -11297,7 +11297,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>10</v>
       </c>
@@ -11324,7 +11324,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>6</v>
       </c>
@@ -11351,7 +11351,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>10</v>
       </c>
@@ -11378,7 +11378,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>7</v>
       </c>
@@ -11405,7 +11405,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>10</v>
       </c>
@@ -11432,7 +11432,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>6</v>
       </c>
@@ -11459,7 +11459,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>10</v>
       </c>
@@ -11486,7 +11486,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>7</v>
       </c>
@@ -11513,7 +11513,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>10</v>
       </c>
@@ -11540,7 +11540,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>10</v>
       </c>
@@ -11567,7 +11567,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>6</v>
       </c>
@@ -11594,7 +11594,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
@@ -11621,7 +11621,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>10</v>
       </c>
@@ -11648,7 +11648,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>10</v>
       </c>
@@ -11675,7 +11675,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>6</v>
       </c>
@@ -11702,7 +11702,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
@@ -11729,7 +11729,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>10</v>
       </c>
@@ -11756,7 +11756,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>6</v>
       </c>
@@ -11783,7 +11783,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>10</v>
       </c>
@@ -11810,7 +11810,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>7</v>
       </c>
@@ -11837,7 +11837,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>10</v>
       </c>
@@ -11864,7 +11864,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>6</v>
       </c>
@@ -11891,7 +11891,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>10</v>
       </c>
@@ -11918,7 +11918,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>7</v>
       </c>
@@ -11945,7 +11945,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>10</v>
       </c>
@@ -11972,7 +11972,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>6</v>
       </c>
@@ -11999,7 +11999,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>10</v>
       </c>
@@ -12026,7 +12026,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>7</v>
       </c>
@@ -12053,7 +12053,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>10</v>
       </c>
@@ -12080,7 +12080,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>6</v>
       </c>
@@ -12107,7 +12107,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>10</v>
       </c>
@@ -12134,7 +12134,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>7</v>
       </c>
@@ -12161,7 +12161,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>10</v>
       </c>
@@ -12188,7 +12188,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>10</v>
       </c>
@@ -12215,7 +12215,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>6</v>
       </c>
@@ -12242,7 +12242,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>7</v>
       </c>
@@ -12269,7 +12269,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>10</v>
       </c>
@@ -12296,7 +12296,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>10</v>
       </c>
@@ -12323,7 +12323,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>6</v>
       </c>
@@ -12350,7 +12350,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>7</v>
       </c>
@@ -12377,7 +12377,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>10</v>
       </c>
@@ -12404,7 +12404,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>6</v>
       </c>
@@ -12431,7 +12431,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>10</v>
       </c>
@@ -12458,7 +12458,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>7</v>
       </c>
@@ -12485,7 +12485,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>10</v>
       </c>
@@ -12512,7 +12512,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>6</v>
       </c>
@@ -12539,7 +12539,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>10</v>
       </c>
@@ -12566,7 +12566,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>7</v>
       </c>
@@ -12593,7 +12593,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>10</v>
       </c>
@@ -12620,7 +12620,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>6</v>
       </c>
@@ -12647,7 +12647,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>10</v>
       </c>
@@ -12674,7 +12674,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>7</v>
       </c>
@@ -12701,7 +12701,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>10</v>
       </c>
@@ -12728,7 +12728,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>6</v>
       </c>
@@ -12755,7 +12755,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>10</v>
       </c>
@@ -12782,7 +12782,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>7</v>
       </c>
@@ -12809,7 +12809,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>10</v>
       </c>
@@ -12836,7 +12836,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>10</v>
       </c>
@@ -12863,7 +12863,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>6</v>
       </c>
@@ -12890,7 +12890,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>7</v>
       </c>
@@ -12917,7 +12917,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>10</v>
       </c>
@@ -12944,7 +12944,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>10</v>
       </c>
@@ -12971,7 +12971,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>6</v>
       </c>
@@ -12998,7 +12998,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>7</v>
       </c>
@@ -13025,7 +13025,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>10</v>
       </c>
@@ -13052,7 +13052,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>6</v>
       </c>
@@ -13079,7 +13079,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>10</v>
       </c>
@@ -13106,7 +13106,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>7</v>
       </c>
@@ -13133,7 +13133,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>10</v>
       </c>
@@ -13160,7 +13160,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>6</v>
       </c>
@@ -13187,7 +13187,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>10</v>
       </c>
@@ -13214,7 +13214,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>7</v>
       </c>
@@ -13241,7 +13241,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>10</v>
       </c>
@@ -13268,7 +13268,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>6</v>
       </c>
@@ -13295,7 +13295,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>10</v>
       </c>
@@ -13322,7 +13322,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>7</v>
       </c>
@@ -13349,7 +13349,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>10</v>
       </c>
@@ -13376,7 +13376,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>6</v>
       </c>
@@ -13403,7 +13403,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>10</v>
       </c>
@@ -13430,7 +13430,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>7</v>
       </c>
@@ -13457,7 +13457,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>10</v>
       </c>
@@ -13484,7 +13484,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>10</v>
       </c>
@@ -13511,7 +13511,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>6</v>
       </c>
@@ -13538,7 +13538,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>7</v>
       </c>
@@ -13565,7 +13565,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>10</v>
       </c>
@@ -13592,7 +13592,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>10</v>
       </c>
@@ -13619,7 +13619,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>6</v>
       </c>
@@ -13646,7 +13646,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>7</v>
       </c>
@@ -13673,7 +13673,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>10</v>
       </c>
@@ -13700,7 +13700,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>6</v>
       </c>
@@ -13727,7 +13727,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>10</v>
       </c>
@@ -13754,7 +13754,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>7</v>
       </c>
@@ -13781,7 +13781,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>10</v>
       </c>
@@ -13808,7 +13808,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>6</v>
       </c>
@@ -13835,7 +13835,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>10</v>
       </c>
@@ -13862,7 +13862,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>7</v>
       </c>
@@ -13889,7 +13889,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>10</v>
       </c>
@@ -13916,7 +13916,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>6</v>
       </c>
@@ -13943,7 +13943,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>10</v>
       </c>
@@ -13970,7 +13970,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>7</v>
       </c>
@@ -13997,7 +13997,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>10</v>
       </c>
@@ -14024,7 +14024,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>6</v>
       </c>
@@ -14051,7 +14051,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>10</v>
       </c>
@@ -14078,7 +14078,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>7</v>
       </c>
@@ -14105,7 +14105,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>10</v>
       </c>
@@ -14132,7 +14132,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>10</v>
       </c>
@@ -14159,7 +14159,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>6</v>
       </c>
@@ -14186,7 +14186,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>7</v>
       </c>
@@ -14213,7 +14213,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>10</v>
       </c>
@@ -14240,7 +14240,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>10</v>
       </c>
@@ -14267,7 +14267,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>6</v>
       </c>
@@ -14294,7 +14294,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>7</v>
       </c>
@@ -14321,7 +14321,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>10</v>
       </c>
@@ -14348,7 +14348,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>6</v>
       </c>
@@ -14375,7 +14375,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>10</v>
       </c>
@@ -14402,7 +14402,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>7</v>
       </c>
@@ -14429,7 +14429,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
         <v>10</v>
       </c>
@@ -14456,7 +14456,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
         <v>6</v>
       </c>
@@ -14483,7 +14483,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
         <v>10</v>
       </c>
@@ -14510,7 +14510,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
         <v>7</v>
       </c>
@@ -14537,7 +14537,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
         <v>10</v>
       </c>
@@ -14564,7 +14564,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
         <v>6</v>
       </c>
@@ -14591,7 +14591,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
         <v>10</v>
       </c>
@@ -14618,7 +14618,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
         <v>7</v>
       </c>
@@ -14645,7 +14645,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
         <v>10</v>
       </c>
@@ -14672,7 +14672,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
         <v>6</v>
       </c>
@@ -14699,7 +14699,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
         <v>10</v>
       </c>
@@ -14726,7 +14726,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
         <v>7</v>
       </c>
@@ -14753,7 +14753,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>10</v>
       </c>
@@ -14789,19 +14789,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A230560C-415B-4967-8544-DB47483911E3}">
   <dimension ref="A1:F193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -14821,7 +14821,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -14838,7 +14838,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -14855,7 +14855,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -14872,7 +14872,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -14892,7 +14892,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -14909,7 +14909,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -14926,7 +14926,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -14943,7 +14943,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -14963,7 +14963,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -14980,7 +14980,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -15000,7 +15000,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -15017,7 +15017,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -15034,7 +15034,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -15051,7 +15051,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -15068,7 +15068,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -15085,7 +15085,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -15102,7 +15102,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -15122,7 +15122,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -15142,7 +15142,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -15159,7 +15159,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -15179,7 +15179,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -15196,7 +15196,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -15216,7 +15216,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -15233,7 +15233,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -15253,7 +15253,7 @@
         <v>44727</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -15273,7 +15273,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -15293,7 +15293,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -15313,7 +15313,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -15333,7 +15333,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -15350,7 +15350,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -15367,7 +15367,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -15384,7 +15384,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -15401,7 +15401,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
@@ -15418,7 +15418,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -15435,7 +15435,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -15452,7 +15452,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -15472,7 +15472,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -15489,7 +15489,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
@@ -15509,7 +15509,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
@@ -15526,7 +15526,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -15543,7 +15543,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
@@ -15560,7 +15560,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -15577,7 +15577,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
@@ -15594,7 +15594,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
@@ -15614,7 +15614,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
@@ -15634,7 +15634,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
@@ -15654,7 +15654,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -15671,7 +15671,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
@@ -15691,7 +15691,7 @@
         <v>44741</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
@@ -15708,7 +15708,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>6</v>
       </c>
@@ -15725,7 +15725,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -15742,7 +15742,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
@@ -15759,7 +15759,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>10</v>
       </c>
@@ -15776,7 +15776,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>6</v>
       </c>
@@ -15793,7 +15793,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -15810,7 +15810,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>10</v>
       </c>
@@ -15827,7 +15827,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>6</v>
       </c>
@@ -15844,7 +15844,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>10</v>
       </c>
@@ -15861,7 +15861,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -15878,7 +15878,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>10</v>
       </c>
@@ -15895,7 +15895,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>6</v>
       </c>
@@ -15912,7 +15912,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>10</v>
       </c>
@@ -15929,7 +15929,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -15946,7 +15946,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>10</v>
       </c>
@@ -15963,7 +15963,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>6</v>
       </c>
@@ -15980,7 +15980,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>10</v>
       </c>
@@ -15997,7 +15997,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>7</v>
       </c>
@@ -16014,7 +16014,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>10</v>
       </c>
@@ -16031,7 +16031,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>6</v>
       </c>
@@ -16048,7 +16048,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>10</v>
       </c>
@@ -16065,7 +16065,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>7</v>
       </c>
@@ -16082,7 +16082,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>10</v>
       </c>
@@ -16102,7 +16102,7 @@
         <v>44755</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>10</v>
       </c>
@@ -16119,7 +16119,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>6</v>
       </c>
@@ -16136,7 +16136,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
@@ -16153,7 +16153,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>10</v>
       </c>
@@ -16170,7 +16170,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>10</v>
       </c>
@@ -16187,7 +16187,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>6</v>
       </c>
@@ -16204,7 +16204,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
@@ -16221,7 +16221,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>10</v>
       </c>
@@ -16238,7 +16238,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>6</v>
       </c>
@@ -16255,7 +16255,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>10</v>
       </c>
@@ -16272,7 +16272,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>7</v>
       </c>
@@ -16289,7 +16289,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>10</v>
       </c>
@@ -16306,7 +16306,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>6</v>
       </c>
@@ -16323,7 +16323,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>10</v>
       </c>
@@ -16340,7 +16340,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>7</v>
       </c>
@@ -16357,7 +16357,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>10</v>
       </c>
@@ -16374,7 +16374,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>6</v>
       </c>
@@ -16391,7 +16391,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>10</v>
       </c>
@@ -16408,7 +16408,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>7</v>
       </c>
@@ -16425,7 +16425,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>10</v>
       </c>
@@ -16442,7 +16442,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>6</v>
       </c>
@@ -16459,7 +16459,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>10</v>
       </c>
@@ -16476,7 +16476,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>7</v>
       </c>
@@ -16493,7 +16493,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>10</v>
       </c>
@@ -16510,7 +16510,7 @@
         <v>44769</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>10</v>
       </c>
@@ -16527,7 +16527,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>6</v>
       </c>
@@ -16544,7 +16544,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>7</v>
       </c>
@@ -16561,7 +16561,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>10</v>
       </c>
@@ -16578,7 +16578,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>10</v>
       </c>
@@ -16595,7 +16595,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>6</v>
       </c>
@@ -16612,7 +16612,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>7</v>
       </c>
@@ -16629,7 +16629,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>10</v>
       </c>
@@ -16646,7 +16646,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>6</v>
       </c>
@@ -16663,7 +16663,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>10</v>
       </c>
@@ -16680,7 +16680,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>7</v>
       </c>
@@ -16697,7 +16697,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>10</v>
       </c>
@@ -16714,7 +16714,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>6</v>
       </c>
@@ -16731,7 +16731,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>10</v>
       </c>
@@ -16748,7 +16748,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>7</v>
       </c>
@@ -16765,7 +16765,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>10</v>
       </c>
@@ -16782,7 +16782,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>6</v>
       </c>
@@ -16799,7 +16799,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>10</v>
       </c>
@@ -16816,7 +16816,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>7</v>
       </c>
@@ -16833,7 +16833,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>10</v>
       </c>
@@ -16850,7 +16850,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>6</v>
       </c>
@@ -16867,7 +16867,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>10</v>
       </c>
@@ -16884,7 +16884,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>7</v>
       </c>
@@ -16901,7 +16901,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>10</v>
       </c>
@@ -16918,7 +16918,7 @@
         <v>44784</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>10</v>
       </c>
@@ -16935,7 +16935,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>6</v>
       </c>
@@ -16952,7 +16952,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>7</v>
       </c>
@@ -16969,7 +16969,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>10</v>
       </c>
@@ -16986,7 +16986,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>10</v>
       </c>
@@ -17003,7 +17003,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>6</v>
       </c>
@@ -17023,7 +17023,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>7</v>
       </c>
@@ -17040,7 +17040,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>10</v>
       </c>
@@ -17057,7 +17057,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>6</v>
       </c>
@@ -17074,7 +17074,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>10</v>
       </c>
@@ -17091,7 +17091,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>7</v>
       </c>
@@ -17108,7 +17108,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>10</v>
       </c>
@@ -17125,7 +17125,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>6</v>
       </c>
@@ -17142,7 +17142,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>10</v>
       </c>
@@ -17159,7 +17159,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>7</v>
       </c>
@@ -17176,7 +17176,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>10</v>
       </c>
@@ -17193,7 +17193,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>6</v>
       </c>
@@ -17210,7 +17210,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>10</v>
       </c>
@@ -17227,7 +17227,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>7</v>
       </c>
@@ -17244,7 +17244,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>10</v>
       </c>
@@ -17261,7 +17261,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>6</v>
       </c>
@@ -17278,7 +17278,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>10</v>
       </c>
@@ -17295,7 +17295,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>7</v>
       </c>
@@ -17312,7 +17312,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>10</v>
       </c>
@@ -17329,7 +17329,7 @@
         <v>44796</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>10</v>
       </c>
@@ -17346,7 +17346,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>6</v>
       </c>
@@ -17363,7 +17363,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>7</v>
       </c>
@@ -17380,7 +17380,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>10</v>
       </c>
@@ -17397,7 +17397,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>10</v>
       </c>
@@ -17414,7 +17414,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>6</v>
       </c>
@@ -17431,7 +17431,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>7</v>
       </c>
@@ -17448,7 +17448,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>10</v>
       </c>
@@ -17465,7 +17465,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>6</v>
       </c>
@@ -17482,7 +17482,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>10</v>
       </c>
@@ -17499,7 +17499,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>7</v>
       </c>
@@ -17516,7 +17516,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>10</v>
       </c>
@@ -17533,7 +17533,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>6</v>
       </c>
@@ -17550,7 +17550,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>10</v>
       </c>
@@ -17567,7 +17567,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>7</v>
       </c>
@@ -17584,7 +17584,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>10</v>
       </c>
@@ -17601,7 +17601,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>6</v>
       </c>
@@ -17618,7 +17618,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>10</v>
       </c>
@@ -17635,7 +17635,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>7</v>
       </c>
@@ -17652,7 +17652,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>10</v>
       </c>
@@ -17669,7 +17669,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>6</v>
       </c>
@@ -17686,7 +17686,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>10</v>
       </c>
@@ -17703,7 +17703,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>7</v>
       </c>
@@ -17720,7 +17720,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>10</v>
       </c>
@@ -17737,7 +17737,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>10</v>
       </c>
@@ -17754,7 +17754,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>6</v>
       </c>
@@ -17771,7 +17771,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>7</v>
       </c>
@@ -17788,7 +17788,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>10</v>
       </c>
@@ -17805,7 +17805,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>10</v>
       </c>
@@ -17822,7 +17822,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>6</v>
       </c>
@@ -17839,7 +17839,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>7</v>
       </c>
@@ -17856,7 +17856,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>10</v>
       </c>
@@ -17876,7 +17876,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>6</v>
       </c>
@@ -17893,7 +17893,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>10</v>
       </c>
@@ -17913,7 +17913,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>7</v>
       </c>
@@ -17930,7 +17930,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
         <v>10</v>
       </c>
@@ -17947,7 +17947,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
         <v>6</v>
       </c>
@@ -17964,7 +17964,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
         <v>10</v>
       </c>
@@ -17981,7 +17981,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
         <v>7</v>
       </c>
@@ -17998,7 +17998,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
         <v>10</v>
       </c>
@@ -18015,7 +18015,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
         <v>6</v>
       </c>
@@ -18032,7 +18032,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
         <v>10</v>
       </c>
@@ -18049,7 +18049,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
         <v>7</v>
       </c>
@@ -18069,7 +18069,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
         <v>10</v>
       </c>
@@ -18089,7 +18089,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
         <v>6</v>
       </c>
@@ -18106,7 +18106,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
         <v>10</v>
       </c>
@@ -18123,7 +18123,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
         <v>7</v>
       </c>
@@ -18140,7 +18140,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>